<commit_message>
Change size to images
</commit_message>
<xml_diff>
--- a/img/weatherImg.xlsx
+++ b/img/weatherImg.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\PowerBI\PB-WeatherApplication\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\PowerBI\PB-Projects\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A3D83B-2952-48C8-8F60-2AEFFFD2795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E405BC-EAAE-44E5-8BB2-337DD1F26D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="690" windowWidth="24240" windowHeight="13140" xr2:uid="{834C1B66-26D2-48C1-A449-B43058D91580}"/>
   </bookViews>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,13 +557,13 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,399 +578,402 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="str" cm="1">
-        <f t="array" aca="1" ref="B2" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A2&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Blizzard.png</v>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2" si="0">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A2&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Blizzard.png</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="str" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A3&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Clear.png</v>
+      <c r="B3" t="str">
+        <f>"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A3&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Clear.png</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="str" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A4&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\CloudRainThunder.png</v>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B45" si="1">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A4&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/CloudRainThunder.png</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="str" cm="1">
-        <f t="array" aca="1" ref="B5" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A5&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\CloudSleetSnowThunder.png</v>
+      <c r="B5" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/CloudSleetSnowThunder.png</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="str" cm="1">
-        <f t="array" aca="1" ref="B6" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A6&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Cloudy.png</v>
+      <c r="B6" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Cloudy.png</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="str" cm="1">
-        <f t="array" aca="1" ref="B7" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A7&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Fog.png</v>
+      <c r="B7" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Fog.png</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="str" cm="1">
-        <f t="array" aca="1" ref="B8" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A8&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\FreezingDrizzle.png</v>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingDrizzle.png</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="str" cm="1">
-        <f t="array" aca="1" ref="B9" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A9&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\FreezingFog.png</v>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingFog.png</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="str" cm="1">
-        <f t="array" aca="1" ref="B10" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A10&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\FreezingRain.png</v>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingRain.png</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="str" cm="1">
-        <f t="array" aca="1" ref="B11" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A11&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavyRain.png</v>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRain.png</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="str" cm="1">
-        <f t="array" aca="1" ref="B12" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A12&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavyRainSwrsDay.png</v>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRainSwrsDay.png</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="str" cm="1">
-        <f t="array" aca="1" ref="B13" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A13&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavyRainSwrsNight.png</v>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRainSwrsNight.png</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="str" cm="1">
-        <f t="array" aca="1" ref="B14" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A14&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySleet.png</v>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleet.png</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="str" cm="1">
-        <f t="array" aca="1" ref="B15" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A15&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySleetSwrsDay.png</v>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleetSwrsDay.png</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="str" cm="1">
-        <f t="array" aca="1" ref="B16" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A16&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySleetSwrsNight.png</v>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleetSwrsNight.png</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="str" cm="1">
-        <f t="array" aca="1" ref="B17" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A17&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySnow.png</v>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnow.png</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="str" cm="1">
-        <f t="array" aca="1" ref="B18" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A18&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySnowSwrsDay.png</v>
+      <c r="B18" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnowSwrsDay.png</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="str" cm="1">
-        <f t="array" aca="1" ref="B19" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A19&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\HeavySnowSwrsNight.png</v>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnowSwrsNight.png</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="str" cm="1">
-        <f t="array" aca="1" ref="B20" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A20&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoRainSwrsDay.png</v>
+      <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoRainSwrsDay.png</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="str" cm="1">
-        <f t="array" aca="1" ref="B21" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A21&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoRainSwrsNight.png</v>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoRainSwrsNight.png</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="str" cm="1">
-        <f t="array" aca="1" ref="B22" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A22&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoSleetSwrsDay.png</v>
+      <c r="B22" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSleetSwrsDay.png</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="str" cm="1">
-        <f t="array" aca="1" ref="B23" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A23&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoSleetSwrsNight.png</v>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSleetSwrsNight.png</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="str" cm="1">
-        <f t="array" aca="1" ref="B24" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A24&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoSnowSwrsDay.png</v>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSnowSwrsDay.png</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="str" cm="1">
-        <f t="array" aca="1" ref="B25" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A25&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\IsoSnowSwrsNight.png</v>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSnowSwrsNight.png</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="str" cm="1">
-        <f t="array" aca="1" ref="B26" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A26&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\mist.png</v>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/mist.png</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="str" cm="1">
-        <f t="array" aca="1" ref="B27" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A27&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModRain.png</v>
+      <c r="B27" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModRain.png</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="str" cm="1">
-        <f t="array" aca="1" ref="B28" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A28&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModRainSwrsDay.png</v>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModRainSwrsDay.png</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="str" cm="1">
-        <f t="array" aca="1" ref="B29" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A29&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSleet.png</v>
+      <c r="B29" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleet.png</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="str" cm="1">
-        <f t="array" aca="1" ref="B30" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A30&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSleetSwrsDay.png</v>
+      <c r="B30" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleetSwrsDay.png</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="str" cm="1">
-        <f t="array" aca="1" ref="B31" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A31&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSleetSwrsNight.png</v>
+      <c r="B31" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleetSwrsNight.png</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="str" cm="1">
-        <f t="array" aca="1" ref="B32" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A32&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSnow.png</v>
+      <c r="B32" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnow.png</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="str" cm="1">
-        <f t="array" aca="1" ref="B33" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A33&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSnowSwrsDay.png</v>
+      <c r="B33" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnowSwrsDay.png</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="str" cm="1">
-        <f t="array" aca="1" ref="B34" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A34&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\ModSnowSwrsNight.png</v>
+      <c r="B34" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnowSwrsNight.png</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="str" cm="1">
-        <f t="array" aca="1" ref="B35" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A35&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\OccLightRain.png</v>
+      <c r="B35" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightRain.png</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="str" cm="1">
-        <f t="array" aca="1" ref="B36" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A36&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\OccLightSleet.png</v>
+      <c r="B36" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightSleet.png</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="str" cm="1">
-        <f t="array" aca="1" ref="B37" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A37&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\OccLightSnow.png</v>
+      <c r="B37" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightSnow.png</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="str" cm="1">
-        <f t="array" aca="1" ref="B38" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A38&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Overcast.png</v>
+      <c r="B38" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Overcast.png</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="str" cm="1">
-        <f t="array" aca="1" ref="B39" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A39&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartCloudRainThunderDay.png</v>
+      <c r="B39" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudRainThunderDay.png</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="str" cm="1">
-        <f t="array" aca="1" ref="B40" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A40&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartCloudRainThunderNight.png</v>
+      <c r="B40" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudRainThunderNight.png</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="str" cm="1">
-        <f t="array" aca="1" ref="B41" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A41&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartCloudSleetSnowThunderDay.png</v>
+      <c r="B41" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudSleetSnowThunderDay.png</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="str" cm="1">
-        <f t="array" aca="1" ref="B42" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A42&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartCloudSleetSnowThunderNight.png</v>
+      <c r="B42" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudSleetSnowThunderNight.png</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="str" cm="1">
-        <f t="array" aca="1" ref="B43" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A43&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartlyCloudyDay.png</v>
+      <c r="B43" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartlyCloudyDay.png</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B44" t="str" cm="1">
-        <f t="array" aca="1" ref="B44" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A44&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\PartlyCloudyNight.png</v>
+      <c r="B44" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartlyCloudyNight.png</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-      <c r="B45" t="str" cm="1">
-        <f t="array" aca="1" ref="B45" ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)&amp;A45&amp;".png"</f>
-        <v>C:\Repositories\PowerBI\PB-WeatherApplication\img\Sunny.png</v>
+      <c r="B45" t="str">
+        <f t="shared" si="1"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Sunny.png</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Blizzard.png" xr:uid="{7CC56E2C-7E02-4063-A622-C0B1E35282EE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to 2 images
</commit_message>
<xml_diff>
--- a/img/weatherImg.xlsx
+++ b/img/weatherImg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\PowerBI\PB-Projects\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E405BC-EAAE-44E5-8BB2-337DD1F26D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018AB4B7-1950-4FB3-9162-649D79121915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="690" windowWidth="24240" windowHeight="13140" xr2:uid="{834C1B66-26D2-48C1-A449-B43058D91580}"/>
   </bookViews>
@@ -44,136 +44,136 @@
     <t>link</t>
   </si>
   <si>
-    <t>Blizzard</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>CloudRainThunder</t>
-  </si>
-  <si>
-    <t>CloudSleetSnowThunder</t>
-  </si>
-  <si>
-    <t>Cloudy</t>
-  </si>
-  <si>
-    <t>Fog</t>
-  </si>
-  <si>
-    <t>FreezingDrizzle</t>
-  </si>
-  <si>
-    <t>FreezingFog</t>
-  </si>
-  <si>
-    <t>FreezingRain</t>
-  </si>
-  <si>
-    <t>HeavyRain</t>
-  </si>
-  <si>
-    <t>HeavyRainSwrsDay</t>
-  </si>
-  <si>
-    <t>HeavyRainSwrsNight</t>
-  </si>
-  <si>
-    <t>HeavySleet</t>
-  </si>
-  <si>
-    <t>HeavySleetSwrsDay</t>
-  </si>
-  <si>
-    <t>HeavySleetSwrsNight</t>
-  </si>
-  <si>
-    <t>HeavySnow</t>
-  </si>
-  <si>
-    <t>HeavySnowSwrsDay</t>
-  </si>
-  <si>
-    <t>HeavySnowSwrsNight</t>
-  </si>
-  <si>
-    <t>IsoRainSwrsDay</t>
-  </si>
-  <si>
-    <t>IsoRainSwrsNight</t>
-  </si>
-  <si>
-    <t>IsoSleetSwrsDay</t>
-  </si>
-  <si>
-    <t>IsoSleetSwrsNight</t>
-  </si>
-  <si>
-    <t>IsoSnowSwrsDay</t>
-  </si>
-  <si>
-    <t>IsoSnowSwrsNight</t>
-  </si>
-  <si>
-    <t>mist</t>
-  </si>
-  <si>
-    <t>ModRain</t>
-  </si>
-  <si>
-    <t>ModRainSwrsDay</t>
-  </si>
-  <si>
-    <t>ModSleet</t>
-  </si>
-  <si>
-    <t>ModSleetSwrsDay</t>
-  </si>
-  <si>
-    <t>ModSleetSwrsNight</t>
-  </si>
-  <si>
-    <t>ModSnow</t>
-  </si>
-  <si>
-    <t>ModSnowSwrsDay</t>
-  </si>
-  <si>
-    <t>ModSnowSwrsNight</t>
-  </si>
-  <si>
-    <t>OccLightRain</t>
-  </si>
-  <si>
-    <t>OccLightSleet</t>
-  </si>
-  <si>
-    <t>OccLightSnow</t>
-  </si>
-  <si>
-    <t>Overcast</t>
-  </si>
-  <si>
-    <t>PartCloudRainThunderDay</t>
-  </si>
-  <si>
-    <t>PartCloudRainThunderNight</t>
-  </si>
-  <si>
-    <t>PartCloudSleetSnowThunderDay</t>
-  </si>
-  <si>
-    <t>PartCloudSleetSnowThunderNight</t>
-  </si>
-  <si>
-    <t>PartlyCloudyDay</t>
-  </si>
-  <si>
-    <t>PartlyCloudyNight</t>
-  </si>
-  <si>
-    <t>Sunny</t>
+    <t>Blizzard.gif</t>
+  </si>
+  <si>
+    <t>Clear.gif</t>
+  </si>
+  <si>
+    <t>CloudRainThunder.gif</t>
+  </si>
+  <si>
+    <t>CloudSleetSnowThunder.gif</t>
+  </si>
+  <si>
+    <t>Cloudy.gif</t>
+  </si>
+  <si>
+    <t>Fog.gif</t>
+  </si>
+  <si>
+    <t>FreezingDrizzle.gif</t>
+  </si>
+  <si>
+    <t>FreezingFog.gif</t>
+  </si>
+  <si>
+    <t>FreezingRain.gif</t>
+  </si>
+  <si>
+    <t>HeavyRain.gif</t>
+  </si>
+  <si>
+    <t>HeavyRainSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>HeavyRainSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>HeavySleet.gif</t>
+  </si>
+  <si>
+    <t>HeavySleetSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>HeavySleetSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>HeavySnow.gif</t>
+  </si>
+  <si>
+    <t>HeavySnowSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>HeavySnowSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>IsoRainSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>IsoRainSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>IsoSleetSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>IsoSleetSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>IsoSnowSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>IsoSnowSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>mist.gif</t>
+  </si>
+  <si>
+    <t>ModRain.gif</t>
+  </si>
+  <si>
+    <t>ModRainSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>ModSleet.gif</t>
+  </si>
+  <si>
+    <t>ModSleetSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>ModSleetSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>ModSnow.gif</t>
+  </si>
+  <si>
+    <t>ModSnowSwrsDay.gif</t>
+  </si>
+  <si>
+    <t>ModSnowSwrsNight.gif</t>
+  </si>
+  <si>
+    <t>OccLightRain.gif</t>
+  </si>
+  <si>
+    <t>OccLightSleet.gif</t>
+  </si>
+  <si>
+    <t>OccLightSnow.gif</t>
+  </si>
+  <si>
+    <t>Overcast.gif</t>
+  </si>
+  <si>
+    <t>PartCloudRainThunderDay.gif</t>
+  </si>
+  <si>
+    <t>PartCloudRainThunderNight.gif</t>
+  </si>
+  <si>
+    <t>PartCloudSleetSnowThunderDay.gif</t>
+  </si>
+  <si>
+    <t>PartCloudSleetSnowThunderNight.gif</t>
+  </si>
+  <si>
+    <t>PartlyCloudyDay.gif</t>
+  </si>
+  <si>
+    <t>PartlyCloudyNight.gif</t>
+  </si>
+  <si>
+    <t>Sunny.gif</t>
   </si>
 </sst>
 </file>
@@ -554,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25170FCB-E5E6-435A-93DA-B6BA2101CA16}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +566,7 @@
     <col min="2" max="2" width="123.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,406 +574,579 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2" si="0">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A2&amp;".png"</f>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Blizzard.png</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/"&amp;LEFT(A2,FIND(".gif",A2)-1)&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Blizzard.png</v>
+      </c>
+      <c r="C2" t="str">
+        <f>+A2&amp;".gif"</f>
+        <v>Blizzard.gif.gif</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="str">
-        <f>"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A3&amp;".png"</f>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Clear.png</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B3:B45" si="0">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/"&amp;LEFT(A3,FIND(".gif",A3)-1)&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Clear.png</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C45" si="1">+A3&amp;".gif"</f>
+        <v>Clear.gif.gif</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B45" si="1">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/"&amp;A4&amp;".png"</f>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/CloudRainThunder.png</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/CloudRainThunder.png</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>CloudRainThunder.gif.gif</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/CloudSleetSnowThunder.png</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/CloudSleetSnowThunder.png</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>CloudSleetSnowThunder.gif.gif</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Cloudy.png</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Cloudy.png</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>Cloudy.gif.gif</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Fog.png</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Fog.png</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>Fog.gif.gif</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingDrizzle.png</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingDrizzle.png</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>FreezingDrizzle.gif.gif</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingFog.png</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingFog.png</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>FreezingFog.gif.gif</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/FreezingRain.png</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingRain.png</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>FreezingRain.gif.gif</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRain.png</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRain.png</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavyRain.gif.gif</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRainSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRainSwrsDay.png</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavyRainSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavyRainSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRainSwrsNight.png</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavyRainSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleet.png</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleet.png</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySleet.gif.gif</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleetSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleetSwrsDay.png</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySleetSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySleetSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleetSwrsNight.png</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySleetSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnow.png</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnow.png</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySnow.gif.gif</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnowSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnowSwrsDay.png</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySnowSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/HeavySnowSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnowSwrsNight.png</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>HeavySnowSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoRainSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoRainSwrsDay.png</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoRainSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoRainSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoRainSwrsNight.png</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoRainSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSleetSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSleetSwrsDay.png</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoSleetSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSleetSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSleetSwrsNight.png</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoSleetSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSnowSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSnowSwrsDay.png</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoSnowSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/IsoSnowSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSnowSwrsNight.png</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>IsoSnowSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/mist.png</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/mist.png</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>mist.gif.gif</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModRain.png</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRain.png</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>ModRain.gif.gif</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModRainSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRainSwrsDay.png</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>ModRainSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleet.png</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleet.png</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSleet.gif.gif</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleetSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsDay.png</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSleetSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSleetSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsNight.png</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSleetSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnow.png</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnow.png</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSnow.gif.gif</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnowSwrsDay.png</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsDay.png</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSnowSwrsDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/ModSnowSwrsNight.png</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsNight.png</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>ModSnowSwrsNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightRain.png</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightRain.png</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v>OccLightRain.gif.gif</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightSleet.png</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSleet.png</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>OccLightSleet.gif.gif</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/OccLightSnow.png</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSnow.png</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>OccLightSnow.gif.gif</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Overcast.png</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Overcast.png</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>Overcast.gif.gif</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudRainThunderDay.png</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderDay.png</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>PartCloudRainThunderDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudRainThunderNight.png</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderNight.png</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>PartCloudRainThunderNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudSleetSnowThunderDay.png</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderDay.png</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>PartCloudSleetSnowThunderDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartCloudSleetSnowThunderNight.png</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderNight.png</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="1"/>
+        <v>PartCloudSleetSnowThunderNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartlyCloudyDay.png</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyDay.png</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>PartlyCloudyDay.gif.gif</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/PartlyCloudyNight.png</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyNight.png</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>PartlyCloudyNight.gif.gif</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Sunny.png</v>
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Sunny.png</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="1"/>
+        <v>Sunny.gif.gif</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/PB-WeatherApplication/img/Blizzard.png" xr:uid="{7CC56E2C-7E02-4063-A622-C0B1E35282EE}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cahnges to weather.pbix and create the readme file
</commit_message>
<xml_diff>
--- a/img/weatherImg.xlsx
+++ b/img/weatherImg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\PowerBI\PB-Projects\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018AB4B7-1950-4FB3-9162-649D79121915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BDC971-60AE-461F-80F6-87BC7A45B764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="690" windowWidth="24240" windowHeight="13140" xr2:uid="{834C1B66-26D2-48C1-A449-B43058D91580}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>IsoSnowSwrsNight.gif</t>
   </si>
   <si>
-    <t>mist.gif</t>
-  </si>
-  <si>
     <t>ModRain.gif</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Sunny.gif</t>
+  </si>
+  <si>
+    <t>Mist.gif</t>
   </si>
 </sst>
 </file>
@@ -554,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25170FCB-E5E6-435A-93DA-B6BA2101CA16}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +566,7 @@
     <col min="2" max="2" width="123.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -582,12 +582,8 @@
         <f>"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/"&amp;LEFT(A2,FIND(".gif",A2)-1)&amp;".png"</f>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Blizzard.png</v>
       </c>
-      <c r="C2" t="str">
-        <f>+A2&amp;".gif"</f>
-        <v>Blizzard.gif.gif</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -595,12 +591,8 @@
         <f t="shared" ref="B3:B45" si="0">"https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/"&amp;LEFT(A3,FIND(".gif",A3)-1)&amp;".png"</f>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Clear.png</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C45" si="1">+A3&amp;".gif"</f>
-        <v>Clear.gif.gif</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -608,12 +600,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/CloudRainThunder.png</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>CloudRainThunder.gif.gif</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -621,12 +609,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/CloudSleetSnowThunder.png</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>CloudSleetSnowThunder.gif.gif</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -634,12 +618,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Cloudy.png</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="1"/>
-        <v>Cloudy.gif.gif</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -647,12 +627,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Fog.png</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>Fog.gif.gif</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -660,12 +636,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingDrizzle.png</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>FreezingDrizzle.gif.gif</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -673,12 +645,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingFog.png</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>FreezingFog.gif.gif</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -686,12 +654,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/FreezingRain.png</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>FreezingRain.gif.gif</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -699,12 +663,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRain.png</v>
       </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavyRain.gif.gif</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -712,12 +672,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRainSwrsDay.png</v>
       </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavyRainSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -725,12 +681,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavyRainSwrsNight.png</v>
       </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavyRainSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -738,12 +690,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleet.png</v>
       </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySleet.gif.gif</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -751,12 +699,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleetSwrsDay.png</v>
       </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySleetSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -764,12 +708,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySleetSwrsNight.png</v>
       </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySleetSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -777,12 +717,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnow.png</v>
       </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySnow.gif.gif</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -790,12 +726,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnowSwrsDay.png</v>
       </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySnowSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -803,12 +735,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/HeavySnowSwrsNight.png</v>
       </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>HeavySnowSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -816,12 +744,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoRainSwrsDay.png</v>
       </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoRainSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -829,12 +753,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoRainSwrsNight.png</v>
       </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoRainSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -842,12 +762,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSleetSwrsDay.png</v>
       </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoSleetSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -855,12 +771,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSleetSwrsNight.png</v>
       </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoSleetSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -868,12 +780,8 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSnowSwrsDay.png</v>
       </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoSnowSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -881,269 +789,185 @@
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/IsoSnowSwrsNight.png</v>
       </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
-        <v>IsoSnowSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Mist.png</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/mist.png</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
-        <v>mist.gif.gif</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRain.png</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRain.png</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="1"/>
-        <v>ModRain.gif.gif</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRainSwrsDay.png</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModRainSwrsDay.png</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="1"/>
-        <v>ModRainSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleet.png</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleet.png</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSleet.gif.gif</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsDay.png</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsDay.png</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSleetSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsNight.png</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSleetSwrsNight.png</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSleetSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnow.png</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnow.png</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSnow.gif.gif</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsDay.png</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsDay.png</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSnowSwrsDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsNight.png</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/ModSnowSwrsNight.png</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="1"/>
-        <v>ModSnowSwrsNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightRain.png</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightRain.png</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" si="1"/>
-        <v>OccLightRain.gif.gif</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSleet.png</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSleet.png</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" si="1"/>
-        <v>OccLightSleet.gif.gif</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSnow.png</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/OccLightSnow.png</v>
-      </c>
-      <c r="C37" t="str">
-        <f t="shared" si="1"/>
-        <v>OccLightSnow.gif.gif</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Overcast.png</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Overcast.png</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" si="1"/>
-        <v>Overcast.gif.gif</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderDay.png</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderDay.png</v>
-      </c>
-      <c r="C39" t="str">
-        <f t="shared" si="1"/>
-        <v>PartCloudRainThunderDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderNight.png</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudRainThunderNight.png</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="1"/>
-        <v>PartCloudRainThunderNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderDay.png</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderDay.png</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v>PartCloudSleetSnowThunderDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderNight.png</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartCloudSleetSnowThunderNight.png</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" si="1"/>
-        <v>PartCloudSleetSnowThunderNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyDay.png</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyDay.png</v>
-      </c>
-      <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v>PartlyCloudyDay.gif.gif</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyNight.png</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/PartlyCloudyNight.png</v>
-      </c>
-      <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v>PartlyCloudyNight.gif.gif</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>https://raw.githubusercontent.com/Eddisonandres/Power-BI-Projects/refs/heads/main/img/Sunny.png</v>
-      </c>
-      <c r="C45" t="str">
-        <f t="shared" si="1"/>
-        <v>Sunny.gif.gif</v>
       </c>
     </row>
   </sheetData>

</xml_diff>